<commit_message>
update database cs code and add python basic
</commit_message>
<xml_diff>
--- a/Excel/Function.xlsx
+++ b/Excel/Function.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\c\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2650765F-D78E-4FE6-9418-066C3ADB5164}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A23D6AE1-02AA-42E7-A201-D1CB24DA2C74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9600" xr2:uid="{9BF3C365-BB38-4B92-AC5A-471291BEC58C}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Domain</t>
   </si>
@@ -106,6 +107,15 @@
   </si>
   <si>
     <t>PSEUDO Code</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>miles</t>
+  </si>
+  <si>
+    <t>miles=0.621371*km</t>
   </si>
 </sst>
 </file>
@@ -186,12 +196,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -507,15 +517,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9541F2A5-DD31-4465-9F0A-992D770227AC}">
-  <dimension ref="F4:P22"/>
+  <dimension ref="F4:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="8" max="8" width="10.90625" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" customWidth="1"/>
     <col min="14" max="14" width="17.1796875" customWidth="1"/>
     <col min="16" max="16" width="18.7265625" customWidth="1"/>
   </cols>
@@ -564,14 +575,14 @@
         <f>2*F7</f>
         <v>2</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="2" t="s">
+      <c r="K7" s="4"/>
+      <c r="L7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -580,22 +591,22 @@
         <v>2</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H10" si="0">2*F8</f>
+        <f>2*F8</f>
         <v>4</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -604,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f>2*F9</f>
         <v>6</v>
       </c>
       <c r="J9">
@@ -626,7 +637,7 @@
         <v>4</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f>2*F10</f>
         <v>8</v>
       </c>
       <c r="J10">
@@ -636,7 +647,7 @@
         <v>12</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10:M12" si="1">J10*K10</f>
+        <f>J10*K10</f>
         <v>48</v>
       </c>
     </row>
@@ -648,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="M11">
-        <f t="shared" si="1"/>
+        <f>J11*K11</f>
         <v>42</v>
       </c>
       <c r="O11">
@@ -666,13 +677,13 @@
         <v>9</v>
       </c>
       <c r="M12">
-        <f t="shared" si="1"/>
+        <f>J12*K12</f>
         <v>72</v>
       </c>
       <c r="O12">
         <v>2</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -745,7 +756,7 @@
         <v>6</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20:M22" si="2">M10*K20</f>
+        <f>M10*K20</f>
         <v>288</v>
       </c>
     </row>
@@ -754,7 +765,7 @@
         <v>22</v>
       </c>
       <c r="M21">
-        <f t="shared" si="2"/>
+        <f>M11*K21</f>
         <v>924</v>
       </c>
     </row>
@@ -763,8 +774,84 @@
         <v>55</v>
       </c>
       <c r="M22">
-        <f t="shared" si="2"/>
+        <f>M12*K22</f>
         <v>3960</v>
+      </c>
+    </row>
+    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28">
+        <v>0.62137100000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ref="L29:L34" si="0">J29*0.621371</f>
+        <v>1.242742</v>
+      </c>
+    </row>
+    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J30">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>1.8641130000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>2.485484</v>
+      </c>
+    </row>
+    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>3.1068549999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="10:12" x14ac:dyDescent="0.35">
+      <c r="J33">
+        <v>6</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>3.7282260000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="10:12" x14ac:dyDescent="0.35">
+      <c r="J34">
+        <v>25</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>15.534275000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>